<commit_message>
parameterized class and topology
</commit_message>
<xml_diff>
--- a/testplan.xlsx
+++ b/testplan.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29108"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1F0998E-77F4-4ED8-A01C-32451CE77F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="feature extraction" sheetId="1" r:id="rId1"/>
+    <sheet name="testplan" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>Chapter</t>
   </si>
@@ -80,17 +80,86 @@
     <t>SUPPORTED</t>
   </si>
   <si>
-    <t>assertions for valid signals after reset</t>
-  </si>
-  <si>
+    <t>assertions to check the valid signals after deasserting reset</t>
+  </si>
+  <si>
+    <t>Assertions to check the handshaking mechanism</t>
+  </si>
+  <si>
+    <t>Single transaction crossing the 4KB address boundary</t>
+  </si>
+  <si>
+    <t>NOT SUPPORTED</t>
+  </si>
+  <si>
+    <t>INCR bursts supports upto 256 transfers.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WRAP bursts supports burst length 2, 4, 8, 16. Does not support unaligned address
+- Early termination of burst is not supported.
+  For write operation, master may deassert all the strobes to reduce the number of data transfer but must complete the transaction.
+  For read operation, master discards the read data but must complete the transaction.
+- In fixed burst, the address is same for every transfer in the burst. Supports unaligned address.
+- INCR supports unaligned address.
+- Supports narrow transfers.
+  For WRAP or INCR burst, different byte lanes are used for each transfer in transaction.
+  For fixed burst, dame byte lanes are used for each transfer in a transaction
+- supports byte invariance
+Responses:
+  OKAY:- normal access success. can also indicate exclusive access fail.
+  </t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">3.2 </t>
+      <t>EXOKAY:- Exclusive access successful.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  SLVERR:- slave error.
+  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DECERR:- decode error. typically by an interconnect to indicate there is no slave at the transaction address.</t>
+    </r>
+  </si>
+  <si>
+    <t>Transaction Attributes</t>
+  </si>
+  <si>
+    <t>4.1 Transaction types and attributes
+4.2 AXI3 memory attribute signaling
+4.3 AXI4 changes to memory attribute signaling
+4.4 Memory types
+4.5 Mismatched memory attributes
+4.6 Transaction buffering
+4.7 Access permissions
+4.8 Legacy considerations</t>
+  </si>
+  <si>
+    <t>Multiple Transactions</t>
+  </si>
+  <si>
+    <r>
+      <t>3.2 Basic read and write transactions</t>
     </r>
     <r>
       <rPr>
@@ -100,7 +169,7 @@
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Basic read and write transactions
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -110,18 +179,214 @@
         <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t>3.2.1 Handshake process
-source generates  VALID signal to indicate that address, data or control information is available. 
-destination generates the READY signal to indicate that it can
-accept the information</t>
+      <t xml:space="preserve">3.2.1 Handshake process
+source generates  VALID signal to indicate that address, data or control information is available. destination generates the READY signal to indicate that it can
+accept the information.
+- READY signal is independent signal and can be asserted before, after or at the same time address channel signals are asserted.
+-write/read address channel should remain constant until handshaking is completed.
+</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3.3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Relationship between the channels</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Write address channel and write data channel is independent of each other but write response channel signals can be asserted only after the completion of transaction.
+-For write operation, RESP channel signals must come only after the completion of transaction.
+-For read operation, response signals should be asserted alog with each data transfer of the transaction.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3.4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Transaction structure</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Master only provides the starting address of the transaction.
+- Burst transaction must not cross 4KB address boundary.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>5.1 AXI transaction identifiers
+- AXI uses tranaction IDs to identify the transaction and due to this it supports out-of-order transactions.</t>
+  </si>
+  <si>
+    <t>5.3 Transaction ordering
+5.3.1 Read ordering
+- slave must read the data in the order it received addresses for the transaction with same ARID.
+- slave may read thedata in any order for the addesses with the different ARID.</t>
+  </si>
+  <si>
+    <t>5.3.3 AXI3 write data interleaving
+- slave can accept write data with different AWID values.
+- write data from different transactions of same AWID cannot be interleaved.
+- slave should receive the first write data for each transaction in the same roder in which it receives the addresses for transactions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.3.4 Read and write interaction
+- no order restriction between read and write transaction even though values of ARID and AWID is same.
+</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>What to generate</t>
+  </si>
+  <si>
+    <t>What to detect</t>
+  </si>
+  <si>
+    <t>Checker name</t>
+  </si>
+  <si>
+    <t>What to Cover</t>
+  </si>
+  <si>
+    <t>Cover group</t>
+  </si>
+  <si>
+    <t>Feature Reference</t>
+  </si>
+  <si>
+    <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>Error Type</t>
+  </si>
+  <si>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Sr. No.</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Review Status</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Initial Review</t>
+  </si>
+  <si>
+    <t>Review Comments</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Testcase type: Errorneous/ Normal</t>
+  </si>
+  <si>
+    <t>Status: 
+Not Started/ 
+In Progress/ Implemented</t>
+  </si>
+  <si>
+    <t>AXI3/4</t>
+  </si>
+  <si>
+    <t>axi_initial_reset_test</t>
+  </si>
+  <si>
+    <t>Perform an initial reset operation at the begining of the simulation</t>
+  </si>
+  <si>
+    <t>NORMAL</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>1) Apply initial reset at the start of the simulation</t>
+  </si>
+  <si>
+    <t>1) Detect the initial behaviour of slave and initial values of the registers</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>PENDING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,13 +397,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -151,7 +416,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -167,8 +432,56 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,8 +510,36 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC4D79B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -236,14 +577,135 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -278,18 +740,101 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50"/>
+    <cellStyle name="Accent2" xfId="5" builtinId="33"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,7 +895,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -402,7 +947,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -616,33 +1161,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="10" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="17.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="13.25" style="10" customWidth="1"/>
+    <col min="5" max="5" width="18.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.875" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="13" customFormat="1" ht="29.25">
+    <row r="1" spans="1:7" s="12" customFormat="1" ht="30">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -661,7 +1204,7 @@
       <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="19" t="s">
         <v>6</v>
       </c>
     </row>
@@ -671,9 +1214,10 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="57.75">
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="3" spans="1:7" ht="57">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -687,7 +1231,8 @@
         <v>9</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2"/>
@@ -695,7 +1240,8 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
@@ -705,7 +1251,8 @@
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
@@ -713,10 +1260,11 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="101.25">
-      <c r="A7" s="4" t="s">
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" ht="71.25">
+      <c r="A7" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -729,124 +1277,788 @@
         <v>13</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="16"/>
+      <c r="G7" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="115.5">
-      <c r="A8" s="4"/>
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:7" ht="183.75" customHeight="1">
+      <c r="A8" s="24"/>
+      <c r="B8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7" ht="149.25" customHeight="1">
+      <c r="A9" s="24"/>
+      <c r="B9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+    </row>
+    <row r="10" spans="1:7" ht="81" customHeight="1">
+      <c r="A10" s="24"/>
+      <c r="B10" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="F10" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:7" ht="28.5">
+      <c r="A11" s="24"/>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:7" ht="357" customHeight="1">
+      <c r="A12" s="24"/>
+      <c r="B12" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:7" ht="122.25" customHeight="1">
+      <c r="A13" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>21</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:7" ht="57">
+      <c r="A14" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" ht="85.5">
+      <c r="A15" s="32"/>
+      <c r="B15" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" ht="114">
+      <c r="A16" s="32"/>
+      <c r="B16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:7" ht="71.25">
+      <c r="A17" s="29"/>
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A7:A12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1"/>
+    <col min="5" max="5" width="15.75" customWidth="1"/>
+    <col min="6" max="6" width="13.625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="23.5" customWidth="1"/>
+    <col min="9" max="9" width="24.875" customWidth="1"/>
+    <col min="13" max="13" width="13.375" customWidth="1"/>
+    <col min="15" max="15" width="16.25" customWidth="1"/>
+    <col min="17" max="17" width="10.75" customWidth="1"/>
+    <col min="19" max="19" width="12.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="47.25">
+      <c r="A1" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="U1" s="33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="63">
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+    </row>
+    <row r="3" spans="1:21" ht="57">
+      <c r="A3" s="40">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="36"/>
+      <c r="O3" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
+      <c r="U3" s="36"/>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="40">
+        <v>2</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="37"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="36"/>
+      <c r="T5" s="36"/>
+      <c r="U5" s="36"/>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="37"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="37"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="36"/>
+      <c r="S7" s="36"/>
+      <c r="T7" s="36"/>
+      <c r="U7" s="36"/>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="37"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="36"/>
+      <c r="T8" s="36"/>
+      <c r="U8" s="36"/>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="37"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="36"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="36"/>
+      <c r="U9" s="36"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="37"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="36"/>
+      <c r="U10" s="36"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="37"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="36"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="36"/>
+      <c r="U11" s="36"/>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="37"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="37"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="37"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="36"/>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="37"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="36"/>
+      <c r="U15" s="36"/>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="37"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="36"/>
+      <c r="U16" s="36"/>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" s="37"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+    </row>
+    <row r="18" spans="1:21">
+      <c r="A18" s="37"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="36"/>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="37"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="36"/>
+      <c r="U19" s="36"/>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" s="37"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="36"/>
+      <c r="U20" s="36"/>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" s="37"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>